<commit_message>
Versão antes correção ortográfica
</commit_message>
<xml_diff>
--- a/referencias/Controle_Referencias.xlsx
+++ b/referencias/Controle_Referencias.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>#</t>
   </si>
@@ -63,7 +63,7 @@
   </si>
   <si>
     <t>A Systematic Review of Cross- vs. Within-
-Company Cost Estimation Studies </t>
+Company Cost Estimation Studies</t>
   </si>
   <si>
     <t>Exemplo canônico de Revisão Sistemática</t>
@@ -74,7 +74,7 @@
   <si>
     <t>Forecasting of Software De
 velopment Work Effort: 
-Evidence on Expert Judgment and Formal Models </t>
+Evidence on Expert Judgment and Formal Models</t>
   </si>
   <si>
     <t>06-SLR_of_SLR.pdf</t>
@@ -94,7 +94,18 @@
 Engineering</t>
   </si>
   <si>
-    <t>Relatório técnico sobre SLR em Engenharia de Software que propõe um conjunto de diretrizes </t>
+    <t>Relatório técnico sobre SLR em Engenharia de Software que propõe um conjunto de diretrizes</t>
+  </si>
+  <si>
+    <t>08-BTH2012Yasin.pdf</t>
+  </si>
+  <si>
+    <t>On the quality of grey literature and its use
+in information synthesis
+during systematic literature reviews</t>
+  </si>
+  <si>
+    <t>Relatório de uma tese de mestrado sobre a utilização de “grey literature” em revisão sistemática</t>
   </si>
 </sst>
 </file>
@@ -110,6 +121,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -131,6 +143,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -222,13 +235,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="B1:E13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -352,13 +365,19 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="C9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="3" t="n">

</xml_diff>